<commit_message>
finishing shift pattern in admin view
</commit_message>
<xml_diff>
--- a/public/template/template_upload_shiftgroup.xlsx
+++ b/public/template/template_upload_shiftgroup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\ICT - TCF SUPERAPPS\TCF SUPERAPPS\DEVELOPMENT DOCUMENT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\PROJECT TCF 202\tcf-superapps\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A1D816-F1E7-4A8E-84F0-B87AAD546F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D1E7F9-FAF6-4451-BA0F-FFF5BC21599C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BE18CCDD-544B-4E68-8F56-A8F6D4508E88}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>NIK</t>
   </si>
@@ -36,23 +36,47 @@
     <t>NAMA</t>
   </si>
   <si>
-    <t>GRUP ID (SHIFT)</t>
-  </si>
-  <si>
-    <t>Contoh : 093.291018</t>
-  </si>
-  <si>
-    <t>Contoh : ENCEP AB. KOHAR</t>
-  </si>
-  <si>
-    <t>Contoh : 6</t>
+    <t>CURRENT SHIFT</t>
+  </si>
+  <si>
+    <t>PATTERN SHIFT</t>
+  </si>
+  <si>
+    <t>Contoh : 3 Shift</t>
+  </si>
+  <si>
+    <t>BERLAKU SEJAK</t>
+  </si>
+  <si>
+    <t>PATTERN SHIFT ID</t>
+  </si>
+  <si>
+    <t>CURRENT SHIFT ID</t>
+  </si>
+  <si>
+    <t>Contoh : Shift 3 A</t>
+  </si>
+  <si>
+    <t>Contoh : 105.011021</t>
+  </si>
+  <si>
+    <t>Contoh  : RONI SARI MUDA</t>
+  </si>
+  <si>
+    <t>Contoh : 8</t>
+  </si>
+  <si>
+    <t>Contoh : 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,8 +96,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -84,6 +115,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -111,10 +147,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -125,8 +162,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -439,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2977E3-A140-4D1C-962C-CCEBFFF062BE}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,9 +493,12 @@
     <col min="1" max="1" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -462,16 +508,40 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4">
+        <v>45963</v>
       </c>
     </row>
   </sheetData>

</xml_diff>